<commit_message>
Version of CriteriaTaxonomy SELF-CONTAINED for MS revision.
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CriteriaTaxonomy-REGULATED-V2.0.3.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CriteriaTaxonomy-REGULATED-V2.0.3.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11492" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11493" uniqueCount="443">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1375,10 +1375,16 @@
     <t>Where applicable, name of the participating group:</t>
   </si>
   <si>
-    <t>EO_IDENTIFIER</t>
+    <t>51c39ba9-0444-4967-afe9-36f753b30175</t>
   </si>
   <si>
-    <t>Changed in v2.0.3 from DESCRIPTION to IDENTIFIER</t>
+    <t>f4dc58dd-af45-4602-a4c8-3dca30fac082</t>
+  </si>
+  <si>
+    <t>ECONOMIC_OPERATOR_ROLE_CODE</t>
+  </si>
+  <si>
+    <t>Changed in v2.0.3 from DESCRIPTION to ECONOMIC_OPERATOR_ROLE_CODE</t>
   </si>
 </sst>
 </file>
@@ -1542,7 +1548,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1765,6 +1771,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -1957,7 +1969,7 @@
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2332,6 +2344,9 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -15343,7 +15358,9 @@
   <sheetPr codeName="Hoja12"/>
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21465,7 +21482,9 @@
   <sheetPr codeName="Hoja19"/>
   <dimension ref="A1:AX14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S30" sqref="S30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -37115,7 +37134,9 @@
   <sheetPr codeName="Hoja25"/>
   <dimension ref="A1:AX26"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -38517,7 +38538,9 @@
   <sheetPr codeName="Hoja26"/>
   <dimension ref="A1:AX47"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -38722,7 +38745,7 @@
       <c r="W3" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="X3" s="47" t="s">
+      <c r="X3" s="124" t="s">
         <v>276</v>
       </c>
       <c r="Y3" s="115"/>
@@ -45366,13 +45389,13 @@
         <v>1</v>
       </c>
       <c r="V7" s="145" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="W7" s="100"/>
       <c r="X7" s="101"/>
       <c r="Y7" s="101"/>
-      <c r="Z7" s="145" t="s">
-        <v>440</v>
+      <c r="Z7" s="147" t="s">
+        <v>442</v>
       </c>
       <c r="AA7"/>
       <c r="AB7"/>
@@ -52464,7 +52487,9 @@
   <sheetPr codeName="Hoja31"/>
   <dimension ref="A1:AX18"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -54987,7 +55012,9 @@
   <sheetPr codeName="Hoja33"/>
   <dimension ref="A1:AX137"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -56289,7 +56316,9 @@
   <sheetPr codeName="Hoja34"/>
   <dimension ref="A1:AX17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -56479,7 +56508,7 @@
       <c r="U3" s="95"/>
       <c r="V3" s="31"/>
       <c r="W3" s="98" t="s">
-        <v>352</v>
+        <v>439</v>
       </c>
       <c r="X3" s="98" t="s">
         <v>430</v>
@@ -56607,7 +56636,7 @@
       <c r="W5" s="111" t="s">
         <v>422</v>
       </c>
-      <c r="X5" s="99" t="s">
+      <c r="X5" s="28" t="s">
         <v>14</v>
       </c>
       <c r="Y5" s="99"/>
@@ -56681,7 +56710,7 @@
         <v>17</v>
       </c>
       <c r="W6" s="100"/>
-      <c r="X6" s="101" t="s">
+      <c r="X6" s="100" t="s">
         <v>0</v>
       </c>
       <c r="Y6" s="101"/>
@@ -56741,7 +56770,7 @@
       <c r="W7" s="100" t="s">
         <v>423</v>
       </c>
-      <c r="X7" s="101" t="s">
+      <c r="X7" s="100" t="s">
         <v>25</v>
       </c>
       <c r="Y7" s="101"/>
@@ -56799,9 +56828,10 @@
       </c>
       <c r="T8" s="28"/>
       <c r="U8" s="99"/>
-      <c r="V8" s="28"/>
+      <c r="V8" s="100" t="s">
+        <v>29</v>
+      </c>
       <c r="W8" s="100"/>
-      <c r="X8" s="101"/>
       <c r="Y8" s="101"/>
       <c r="Z8" s="28"/>
       <c r="AA8" s="111"/>
@@ -57307,7 +57337,9 @@
   <sheetPr codeName="Hoja35"/>
   <dimension ref="A1:AX13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -57496,7 +57528,7 @@
       <c r="U3" s="95"/>
       <c r="V3" s="31"/>
       <c r="W3" s="98" t="s">
-        <v>352</v>
+        <v>440</v>
       </c>
       <c r="X3" s="98" t="s">
         <v>429</v>

</xml_diff>